<commit_message>
Open Maps API integration
</commit_message>
<xml_diff>
--- a/DATASHEET.xlsx
+++ b/DATASHEET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emanuel Camacho\Documents\Est-gio-ANAC-Emanuel-Camacho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6C945A-976C-442C-AAEC-39F83C3468C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAA1431-269D-482D-A703-B4A1B3C012CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12555" yWindow="2760" windowWidth="12510" windowHeight="8820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fixed" sheetId="2" r:id="rId1"/>
@@ -474,7 +474,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,9 +499,8 @@
       <c r="F1" s="1">
         <v>16</v>
       </c>
-      <c r="G1" s="1">
-        <f>(0.057*0.068)</f>
-        <v>3.8760000000000005E-3</v>
+      <c r="G1">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -524,9 +523,8 @@
       <c r="F2" s="1">
         <v>16</v>
       </c>
-      <c r="G2" s="1">
-        <f t="shared" ref="G2:G19" si="1">(0.057*0.068)</f>
-        <v>3.8760000000000005E-3</v>
+      <c r="G2">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -550,9 +548,8 @@
       <c r="F3" s="1">
         <v>19</v>
       </c>
-      <c r="G3" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G3">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -575,9 +572,8 @@
       <c r="F4" s="1">
         <v>19</v>
       </c>
-      <c r="G4" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G4">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -600,9 +596,8 @@
       <c r="F5" s="1">
         <v>16</v>
       </c>
-      <c r="G5" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G5">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -626,9 +621,8 @@
       <c r="F6" s="1">
         <v>19</v>
       </c>
-      <c r="G6" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G6">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -651,9 +645,8 @@
       <c r="F7" s="1">
         <v>19</v>
       </c>
-      <c r="G7" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G7">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -676,9 +669,8 @@
       <c r="F8" s="1">
         <v>16</v>
       </c>
-      <c r="G8" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G8">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -701,9 +693,8 @@
       <c r="F9" s="1">
         <v>16</v>
       </c>
-      <c r="G9" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G9">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -726,9 +717,8 @@
       <c r="F10" s="1">
         <v>13</v>
       </c>
-      <c r="G10" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G10">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -751,9 +741,8 @@
       <c r="F11" s="1">
         <v>19</v>
       </c>
-      <c r="G11" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G11">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -776,9 +765,8 @@
       <c r="F12" s="1">
         <v>19</v>
       </c>
-      <c r="G12" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G12">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -802,9 +790,8 @@
         <f>(72*1000/3600)</f>
         <v>20</v>
       </c>
-      <c r="G13" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G13">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -828,9 +815,8 @@
         <f>(72*1000/3600)</f>
         <v>20</v>
       </c>
-      <c r="G14" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G14">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -855,9 +841,8 @@
         <f>72*1000/3600</f>
         <v>20</v>
       </c>
-      <c r="G15" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G15">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -881,9 +866,8 @@
         <f>72*1000/3600</f>
         <v>20</v>
       </c>
-      <c r="G16" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G16">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -907,9 +891,8 @@
       <c r="F17" s="1">
         <v>16</v>
       </c>
-      <c r="G17" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G17">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -933,9 +916,8 @@
       <c r="F18" s="1">
         <v>16</v>
       </c>
-      <c r="G18" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G18">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -958,9 +940,8 @@
       <c r="F19" s="1">
         <v>16.5</v>
       </c>
-      <c r="G19" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8760000000000005E-3</v>
+      <c r="G19">
+        <v>6.3454999999999998E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted ballistics and updated data managment
Updated the way horizontal movement worked in a ballistic trajectory via the addition of the side Area parameter separate from top area. Remodelled the way the datasheet is manipulated to prevent data deletion, edit is still not working due to vector dimension missmatch
</commit_message>
<xml_diff>
--- a/DATASHEET.xlsx
+++ b/DATASHEET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emanuel Camacho\Documents\Est-gio-ANAC-Emanuel-Camacho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAA1431-269D-482D-A703-B4A1B3C012CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF130AA4-006B-4818-BF36-13C0EFC251E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12555" yWindow="2760" windowWidth="12510" windowHeight="8820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fixed" sheetId="2" r:id="rId1"/>
@@ -471,15 +471,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -502,8 +502,12 @@
       <c r="G1">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1">
+        <f>(0.058*0.069)</f>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -526,8 +530,12 @@
       <c r="G2">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f t="shared" ref="H2:H19" si="1">(0.058*0.069)</f>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -551,8 +559,12 @@
       <c r="G3">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -575,8 +587,12 @@
       <c r="G4">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -599,8 +615,12 @@
       <c r="G5">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -624,8 +644,12 @@
       <c r="G6">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -648,8 +672,12 @@
       <c r="G7">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -672,8 +700,12 @@
       <c r="G8">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -696,8 +728,12 @@
       <c r="G9">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -720,8 +756,12 @@
       <c r="G10">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -744,8 +784,12 @@
       <c r="G11">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -768,8 +812,12 @@
       <c r="G12">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -793,8 +841,12 @@
       <c r="G13">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -818,8 +870,12 @@
       <c r="G14">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -844,8 +900,12 @@
       <c r="G15">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -869,8 +929,12 @@
       <c r="G16">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -894,8 +958,12 @@
       <c r="G17">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -919,8 +987,12 @@
       <c r="G18">
         <v>6.3454999999999998E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -942,6 +1014,10 @@
       </c>
       <c r="G19">
         <v>6.3454999999999998E-2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>4.0020000000000003E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>